<commit_message>
Added new bom. Fixed mechanical problem.
</commit_message>
<xml_diff>
--- a/Minisumo_EDU_1/Hardware/Minisumo_EDU_1_BOM.xlsx
+++ b/Minisumo_EDU_1/Hardware/Minisumo_EDU_1_BOM.xlsx
@@ -8,12 +8,14 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/zuba1/Documents/Minisumo_Robot_Online_Project/Minisumo_EDU_1/Hardware/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84A58C71-0225-B44B-88A7-25246D0B359F}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E474E2A2-84BA-6949-A646-D084FE5D8F97}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="5020" yWindow="540" windowWidth="24660" windowHeight="18760" xr2:uid="{469D3D62-57C0-F542-B8A2-F47E0700866B}"/>
+    <workbookView xWindow="28800" yWindow="-8180" windowWidth="38400" windowHeight="21600" activeTab="2" xr2:uid="{469D3D62-57C0-F542-B8A2-F47E0700866B}"/>
   </bookViews>
   <sheets>
-    <sheet name="Arkusz1" sheetId="1" r:id="rId1"/>
+    <sheet name="Mainboard_And_Sensors" sheetId="1" r:id="rId1"/>
+    <sheet name="Mechanical" sheetId="2" r:id="rId2"/>
+    <sheet name="TOTAL" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="191029" concurrentCalc="0"/>
   <extLst>
@@ -33,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="97" uniqueCount="82">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="143" uniqueCount="116">
   <si>
     <t>Qty</t>
   </si>
@@ -179,9 +181,6 @@
     <t>https://www.tme.eu/pl/details/smd0805-4k7/rezystory-smd-0805/royal-ohm/0805s8j0472t5e/</t>
   </si>
   <si>
-    <t>Price</t>
-  </si>
-  <si>
     <t>https://www.tme.eu/pl/details/crcw080510k0fktabc/rezystory-smd-0805/vishay/</t>
   </si>
   <si>
@@ -275,17 +274,122 @@
     <t>B+ B-</t>
   </si>
   <si>
-    <t>LiPol</t>
-  </si>
-  <si>
     <t>and create charging cable:</t>
+  </si>
+  <si>
+    <t>LiPol connector</t>
+  </si>
+  <si>
+    <t>PCB</t>
+  </si>
+  <si>
+    <t>Price[PLN]</t>
+  </si>
+  <si>
+    <t>Silicone</t>
+  </si>
+  <si>
+    <t>INSERT 3mm</t>
+  </si>
+  <si>
+    <t>KNIFE</t>
+  </si>
+  <si>
+    <t>Main Board And Sensors</t>
+  </si>
+  <si>
+    <t>Mechanical</t>
+  </si>
+  <si>
+    <t>Robot:</t>
+  </si>
+  <si>
+    <t>Aditional Cost:</t>
+  </si>
+  <si>
+    <t>3d Printing</t>
+  </si>
+  <si>
+    <t>Knife Miling</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Lipol Charger </t>
+  </si>
+  <si>
+    <t>Charging cable</t>
+  </si>
+  <si>
+    <t>TOTAL:</t>
+  </si>
+  <si>
+    <t>Price:</t>
+  </si>
+  <si>
+    <t>Link</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/ladowarka-mikroprocesorowa-redox-alpha-v2-combo-8395806877</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/bateria-li-po-7-4v-2s-500mah-20c-turnigy-rc-7442301257?reco_id=b08b1860-62c0-11ea-b173-246e9680b6a8&amp;sid=041047f9c36843e364ecb91b45c568a2755aa386fe7e14ee7421a14291fbf951</t>
+  </si>
+  <si>
+    <t>Lipol 500mAh 7,4V JST</t>
+  </si>
+  <si>
+    <t>SCREW M3</t>
+  </si>
+  <si>
+    <t>M3x6</t>
+  </si>
+  <si>
+    <t>M3x8</t>
+  </si>
+  <si>
+    <t>M3x15</t>
+  </si>
+  <si>
+    <t>M3x25</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/sruba-kulista-m3-x-25-mm-m3x25-imbus-5-szt-8844405132?bi_s=ads&amp;bi_m=listing%3Adesktop%3Aquery&amp;bi_c=OGUxOTZhZWUtNzFhNy00ODU3LThhMDQtZmU2NzA5Y2VlNTg0AA&amp;bi_t=ape&amp;referrer=proxy&amp;emission_unit_id=3c132aae-6869-4fac-a20c-cf4d1e984cf4</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/sruba-kulista-m3-x-6-mm-m3x6-imbus-5-szt-7290781504?reco_id=99653bda-62c1-11ea-9139-246e964e3280&amp;sid=041047f9c36843e364ecb91b45c568a2755aa386fe7e14ee7421a14291fbf951</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/sruba-kulista-m3-x-16-mm-m3x16-imbus-5-szt-8518838451?reco_id=aeb02152-62c1-11ea-8a86-b02628c85380&amp;sid=1147bbb04b955b96a226cab2e664258d9124ef0862320b2d7366fdd6604cf017</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/metalowa-sruba-ampulowa-din-912-8-8-m3x8mm-10szt-7384599853</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/profesjonalny-silikon-do-form-mm922-0-25kg-polecam-6730393238?snapshot=MjAyMC0wMy0wOVQwNzo1MzoyNi42MTJaO2J1eWVyOzRkOTIzMDhjMTY3ZTNmNDAwNWNlOGM1YzhlMzZmMTczZGViNmJhMzBmNWZjM2Q1MGU5MTM2Y2RjODVhNDcwMzQ%3D</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ALUMINIUM  2mm </t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/insert-gwintowany-m3-7772653476</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/m3-x-5mm-sruba-dociskowa-imbusowa-bez-lba-e8950-8910342394</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/silnik-pololu-mp-30-1-8605570005</t>
+  </si>
+  <si>
+    <t>POLOLU 30:1 MP or HP (or use N20)</t>
+  </si>
+  <si>
+    <t>https://allegro.pl/oferta/noz-do-strugarki-noze-heblarki-ds-ncv1-410x30x3-5894552908</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -322,6 +426,14 @@
       <charset val="238"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <charset val="238"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -344,7 +456,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
@@ -364,6 +476,8 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Hiperłącze" xfId="1" builtinId="8"/>
@@ -681,8 +795,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{80B23C23-568D-3C49-91A8-8823CD668783}">
   <dimension ref="A2:I31"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C33" sqref="C33"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H27" sqref="H27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -697,7 +811,7 @@
   <sheetData>
     <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B2" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
     </row>
     <row r="3" spans="1:9" x14ac:dyDescent="0.2">
@@ -731,7 +845,7 @@
         <v>45</v>
       </c>
       <c r="H4" s="6" t="s">
-        <v>48</v>
+        <v>82</v>
       </c>
       <c r="I4" s="1"/>
     </row>
@@ -782,7 +896,7 @@
         <v>0.05</v>
       </c>
       <c r="H6">
-        <f t="shared" ref="H6:H12" si="0">B6*G6</f>
+        <f t="shared" ref="H6:H13" si="0">B6*G6</f>
         <v>0.05</v>
       </c>
       <c r="I6" s="1"/>
@@ -828,7 +942,7 @@
         <v>11</v>
       </c>
       <c r="F8" s="8" t="s">
-        <v>49</v>
+        <v>48</v>
       </c>
       <c r="G8">
         <v>0.05</v>
@@ -848,13 +962,13 @@
         <v>13</v>
       </c>
       <c r="D9" s="5" t="s">
-        <v>50</v>
+        <v>49</v>
       </c>
       <c r="E9" s="5" t="s">
         <v>14</v>
       </c>
       <c r="F9" s="7" t="s">
-        <v>51</v>
+        <v>50</v>
       </c>
       <c r="G9">
         <v>8.4000000000000005E-2</v>
@@ -880,7 +994,7 @@
         <v>20</v>
       </c>
       <c r="F10" s="8" t="s">
-        <v>52</v>
+        <v>51</v>
       </c>
       <c r="G10">
         <v>0.307</v>
@@ -897,7 +1011,7 @@
         <v>1</v>
       </c>
       <c r="C11" s="5" t="s">
-        <v>53</v>
+        <v>52</v>
       </c>
       <c r="D11" s="5" t="s">
         <v>27</v>
@@ -906,7 +1020,7 @@
         <v>26</v>
       </c>
       <c r="F11" s="8" t="s">
-        <v>54</v>
+        <v>53</v>
       </c>
       <c r="G11">
         <v>3.8</v>
@@ -932,7 +1046,7 @@
         <v>38</v>
       </c>
       <c r="F12" s="8" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="G12">
         <v>2.21</v>
@@ -958,10 +1072,17 @@
         <v>32</v>
       </c>
       <c r="F13" s="8" t="s">
-        <v>63</v>
+        <v>62</v>
+      </c>
+      <c r="G13">
+        <v>0</v>
+      </c>
+      <c r="H13">
+        <f t="shared" si="0"/>
+        <v>0</v>
       </c>
       <c r="I13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
     </row>
     <row r="14" spans="1:9" ht="17" x14ac:dyDescent="0.2">
@@ -970,7 +1091,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="4" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="D14" s="5" t="s">
         <v>7</v>
@@ -979,13 +1100,13 @@
         <v>6</v>
       </c>
       <c r="F14" s="9" t="s">
-        <v>56</v>
+        <v>55</v>
       </c>
       <c r="G14">
         <v>2.16</v>
       </c>
       <c r="H14">
-        <f>B14*G14</f>
+        <f t="shared" ref="H14:H26" si="1">B14*G14</f>
         <v>2.16</v>
       </c>
       <c r="I14" s="1"/>
@@ -996,7 +1117,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="4" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="D15" s="5" t="s">
         <v>5</v>
@@ -1005,13 +1126,13 @@
         <v>4</v>
       </c>
       <c r="F15" s="9" t="s">
-        <v>57</v>
+        <v>56</v>
       </c>
       <c r="G15">
         <v>0.63</v>
       </c>
       <c r="H15">
-        <f>B15*G15</f>
+        <f t="shared" si="1"/>
         <v>1.26</v>
       </c>
       <c r="I15" s="1"/>
@@ -1031,13 +1152,13 @@
         <v>28</v>
       </c>
       <c r="F16" s="8" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="G16">
         <v>0.6</v>
       </c>
       <c r="H16">
-        <f>B16*G16</f>
+        <f t="shared" si="1"/>
         <v>1.2</v>
       </c>
       <c r="I16" s="1"/>
@@ -1054,16 +1175,16 @@
         <v>41</v>
       </c>
       <c r="E17" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F17" s="7" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="G17">
         <v>0.6</v>
       </c>
       <c r="H17">
-        <f>B17*G17</f>
+        <f t="shared" si="1"/>
         <v>2.4</v>
       </c>
     </row>
@@ -1082,13 +1203,13 @@
         <v>40</v>
       </c>
       <c r="F18" s="7" t="s">
-        <v>64</v>
+        <v>63</v>
       </c>
       <c r="G18">
         <v>13</v>
       </c>
       <c r="H18">
-        <f>B18*G18</f>
+        <f t="shared" si="1"/>
         <v>52</v>
       </c>
       <c r="I18" s="1"/>
@@ -1105,16 +1226,16 @@
         <v>36</v>
       </c>
       <c r="E19" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F19" s="10" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G19" s="5">
         <v>0.35</v>
       </c>
       <c r="H19">
-        <f>B19*G19</f>
+        <f t="shared" si="1"/>
         <v>1.4</v>
       </c>
       <c r="I19" s="1"/>
@@ -1134,13 +1255,13 @@
         <v>35</v>
       </c>
       <c r="F20" s="7" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G20">
         <v>16.43</v>
       </c>
       <c r="H20">
-        <f>B20*G20</f>
+        <f t="shared" si="1"/>
         <v>32.86</v>
       </c>
     </row>
@@ -1150,7 +1271,7 @@
         <v>1</v>
       </c>
       <c r="C21" s="4" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="D21" s="5" t="s">
         <v>9</v>
@@ -1159,13 +1280,13 @@
         <v>8</v>
       </c>
       <c r="F21" s="10" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G21">
         <v>15.61</v>
       </c>
       <c r="H21">
-        <f>B21*G21</f>
+        <f t="shared" si="1"/>
         <v>15.61</v>
       </c>
       <c r="I21" s="1"/>
@@ -1182,16 +1303,16 @@
         <v>25</v>
       </c>
       <c r="E22" s="5" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="F22" s="8" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="G22">
         <v>0.72</v>
       </c>
       <c r="H22">
-        <f>B22*G22</f>
+        <f t="shared" si="1"/>
         <v>1.44</v>
       </c>
       <c r="I22" s="1"/>
@@ -1210,13 +1331,13 @@
         <v>24</v>
       </c>
       <c r="F23" s="7" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="G23">
         <v>10</v>
       </c>
       <c r="H23">
-        <f>B23*G23</f>
+        <f t="shared" si="1"/>
         <v>10</v>
       </c>
     </row>
@@ -1234,13 +1355,13 @@
         <v>31</v>
       </c>
       <c r="F24" s="7" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="G24">
         <v>6.42</v>
       </c>
       <c r="H24">
-        <f>B24*G24</f>
+        <f t="shared" si="1"/>
         <v>6.42</v>
       </c>
     </row>
@@ -1249,47 +1370,65 @@
         <v>1</v>
       </c>
       <c r="C25" s="5" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="D25" s="5" t="s">
-        <v>79</v>
+        <v>78</v>
       </c>
       <c r="E25" s="5" t="s">
         <v>80</v>
       </c>
       <c r="F25" s="9" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="G25">
         <v>1</v>
       </c>
       <c r="H25">
-        <f>B25*G25</f>
-        <v>1</v>
+        <f t="shared" si="1"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="B26" s="3">
+        <v>1</v>
+      </c>
+      <c r="C26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="D26" s="5" t="s">
+        <v>81</v>
+      </c>
+      <c r="G26">
+        <v>10</v>
+      </c>
+      <c r="H26">
+        <f t="shared" si="1"/>
+        <v>10</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F27" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="H27">
         <f>SUM(H5:H26)</f>
-        <v>136.11799999999999</v>
+        <v>146.11799999999999</v>
       </c>
     </row>
     <row r="29" spans="1:9" x14ac:dyDescent="0.2">
       <c r="B29" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
     </row>
     <row r="30" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F30" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
     </row>
     <row r="31" spans="1:9" x14ac:dyDescent="0.2">
       <c r="F31" t="s">
-        <v>62</v>
+        <v>61</v>
       </c>
     </row>
   </sheetData>
@@ -1306,4 +1445,325 @@
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{96A5BB3B-4404-F94B-858A-95F32CE791B1}">
+  <dimension ref="C5:F17"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G24" sqref="G24"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="4" max="4" width="38" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="5" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>1</v>
+      </c>
+      <c r="E5" s="6" t="s">
+        <v>43</v>
+      </c>
+      <c r="F5" s="6" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="6" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C6">
+        <v>1</v>
+      </c>
+      <c r="D6" t="s">
+        <v>101</v>
+      </c>
+      <c r="E6" t="s">
+        <v>106</v>
+      </c>
+      <c r="F6">
+        <v>2.13</v>
+      </c>
+    </row>
+    <row r="7" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C7">
+        <v>4</v>
+      </c>
+      <c r="D7" t="s">
+        <v>102</v>
+      </c>
+      <c r="E7" t="s">
+        <v>108</v>
+      </c>
+      <c r="F7">
+        <v>1.2</v>
+      </c>
+    </row>
+    <row r="8" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C8">
+        <v>6</v>
+      </c>
+      <c r="D8" t="s">
+        <v>103</v>
+      </c>
+      <c r="E8" t="s">
+        <v>107</v>
+      </c>
+      <c r="F8">
+        <v>2.56</v>
+      </c>
+    </row>
+    <row r="9" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C9">
+        <v>2</v>
+      </c>
+      <c r="D9" t="s">
+        <v>104</v>
+      </c>
+      <c r="E9" t="s">
+        <v>105</v>
+      </c>
+      <c r="F9">
+        <v>2.4500000000000002</v>
+      </c>
+    </row>
+    <row r="10" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C10">
+        <v>1</v>
+      </c>
+      <c r="D10" t="s">
+        <v>83</v>
+      </c>
+      <c r="E10" t="s">
+        <v>109</v>
+      </c>
+      <c r="F10">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="11" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C11">
+        <v>1</v>
+      </c>
+      <c r="D11" t="s">
+        <v>110</v>
+      </c>
+      <c r="F11">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="12" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C12">
+        <v>2</v>
+      </c>
+      <c r="D12" t="s">
+        <v>84</v>
+      </c>
+      <c r="E12" t="s">
+        <v>111</v>
+      </c>
+      <c r="F12">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="13" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C13">
+        <v>3</v>
+      </c>
+      <c r="D13" t="s">
+        <v>100</v>
+      </c>
+      <c r="E13" t="s">
+        <v>112</v>
+      </c>
+      <c r="F13">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="14" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C14">
+        <v>2</v>
+      </c>
+      <c r="D14" t="s">
+        <v>114</v>
+      </c>
+      <c r="E14" t="s">
+        <v>113</v>
+      </c>
+      <c r="F14">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="15" spans="3:6" x14ac:dyDescent="0.2">
+      <c r="C15">
+        <v>1</v>
+      </c>
+      <c r="D15" t="s">
+        <v>85</v>
+      </c>
+      <c r="E15" t="s">
+        <v>115</v>
+      </c>
+      <c r="F15">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="17" spans="5:6" x14ac:dyDescent="0.2">
+      <c r="E17" t="s">
+        <v>95</v>
+      </c>
+      <c r="F17">
+        <f>SUM(F6:F15)</f>
+        <v>221.34</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E38B9DC8-BC95-9844-86F2-770BDE1BFF91}">
+  <dimension ref="B4:I21"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="25.6640625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="4" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B4" t="s">
+        <v>88</v>
+      </c>
+    </row>
+    <row r="5" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B5" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" t="s">
+        <v>96</v>
+      </c>
+      <c r="D5" s="11" t="s">
+        <v>82</v>
+      </c>
+      <c r="H5" s="12"/>
+      <c r="I5" s="12"/>
+    </row>
+    <row r="6" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B6" t="s">
+        <v>86</v>
+      </c>
+      <c r="D6">
+        <f>Mainboard_And_Sensors!H27</f>
+        <v>146.11799999999999</v>
+      </c>
+    </row>
+    <row r="7" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B7" t="s">
+        <v>87</v>
+      </c>
+      <c r="D7">
+        <f>Mechanical!F17</f>
+        <v>221.34</v>
+      </c>
+    </row>
+    <row r="8" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B8" t="s">
+        <v>99</v>
+      </c>
+      <c r="C8" t="s">
+        <v>98</v>
+      </c>
+      <c r="D8">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="9" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D9">
+        <f>SUM(D6:D8)</f>
+        <v>405.45799999999997</v>
+      </c>
+    </row>
+    <row r="12" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B12" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="13" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B13" s="3" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" t="s">
+        <v>96</v>
+      </c>
+      <c r="D13" s="11" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="14" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B14" t="s">
+        <v>90</v>
+      </c>
+      <c r="D14">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="15" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B15" t="s">
+        <v>91</v>
+      </c>
+      <c r="D15">
+        <v>30</v>
+      </c>
+    </row>
+    <row r="16" spans="2:9" x14ac:dyDescent="0.2">
+      <c r="B16" t="s">
+        <v>92</v>
+      </c>
+      <c r="C16" t="s">
+        <v>97</v>
+      </c>
+      <c r="D16">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="17" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B17" t="s">
+        <v>93</v>
+      </c>
+      <c r="D17">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="18" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B18" t="s">
+        <v>95</v>
+      </c>
+      <c r="D18">
+        <f>SUM(D14:D17)</f>
+        <v>180</v>
+      </c>
+    </row>
+    <row r="21" spans="2:4" x14ac:dyDescent="0.2">
+      <c r="B21" t="s">
+        <v>94</v>
+      </c>
+      <c r="D21">
+        <f>D18+D9</f>
+        <v>585.45799999999997</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>